<commit_message>
Added Vertex and Triangle count graph
</commit_message>
<xml_diff>
--- a/Preliminary Data/50_050_1764097240-Graphed.xlsx
+++ b/Preliminary Data/50_050_1764097240-Graphed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitFork\Comp-302-2202796\COMP302\bin\Debug\net9.0-windows10.0.19041.0\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C93D39E-C021-414A-9C30-E5E1DBEE37A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7780347D-C801-48AB-B0F4-FC22BDBEB9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C0AC00AF-6CA6-4DD7-9918-FEBEAB661DC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C0AC00AF-6CA6-4DD7-9918-FEBEAB661DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="50_050_1764097240" sheetId="1" r:id="rId1"/>
@@ -1952,7 +1952,561 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Vertex and Triangle Counts</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Terrain Generator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$D$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vertex Count</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> Triangle Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50_050_1764097240'!$D$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>674880</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1244160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A4EA-453D-810D-5BCF7F666B70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Quadric Simplification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$D$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vertex Count</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> Triangle Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>701641</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1244148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A4EA-453D-810D-5BCF7F666B70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1559919663"/>
+        <c:axId val="1559914863"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1559919663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1559914863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1559914863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1559919663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2508,6 +3062,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2541,6 +3598,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>69605</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>181706</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>344365</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>73269</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ADE036-F59F-702D-C60C-8A8DDCE32344}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2868,7 +3961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE5CE74-C9F2-4450-A10A-0A480B591D0A}">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -8111,8 +9204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EFDFA6-3EAC-43FB-8076-C79ADDE20907}">
   <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13354,8 +14447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78BA790-5E7D-4543-A39B-EC57BD9C767B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Done a t.test of preliminary data
</commit_message>
<xml_diff>
--- a/Preliminary Data/50_050_1764097240-Graphed.xlsx
+++ b/Preliminary Data/50_050_1764097240-Graphed.xlsx
@@ -5,24 +5,37 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitFork\Comp-302-2202796\COMP302\bin\Debug\net9.0-windows10.0.19041.0\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitFork\Comp-302-2202796\Preliminary Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7780347D-C801-48AB-B0F4-FC22BDBEB9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501DE057-F3A2-4F1C-86D1-8A0EDCF1C983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C0AC00AF-6CA6-4DD7-9918-FEBEAB661DC7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{C0AC00AF-6CA6-4DD7-9918-FEBEAB661DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="50_050_1764097240" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="13">
   <si>
     <t>Seed</t>
   </si>
@@ -58,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Quadric Simplification</t>
+  </si>
+  <si>
+    <t>Average all tiles</t>
   </si>
 </sst>
 </file>
@@ -2466,6 +2482,396 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Average of all Mean</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Geometric Devaition simplifying 50 subdivision mesh by 50%</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$C$164</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Terrain Generator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$B$164</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average all tiles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'50_050_1764097240'!$J$164</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.1222183755987657E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A64-49BA-AE15-69214AAFECAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$164</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Quadric Simplification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'50_050_1764097240'!$B$164</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average all tiles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$164</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2.8784700291666677E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A64-49BA-AE15-69214AAFECAB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1197276207"/>
+        <c:axId val="1197275727"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1197276207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1197275727"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1197275727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1197276207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2507,6 +2913,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3565,6 +4011,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3634,6 +4583,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>525596</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>147044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>114758</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>84155</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8E860D1-9659-4721-631B-D6C1DFE0049D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3959,27 +4944,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE5CE74-C9F2-4450-A10A-0A480B591D0A}">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4011,7 +4996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1764097240</v>
       </c>
@@ -4043,7 +5028,7 @@
         <v>5.3429198000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1764097240</v>
       </c>
@@ -4075,7 +5060,7 @@
         <v>1.5990176999999999E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1764097240</v>
       </c>
@@ -4107,7 +5092,7 @@
         <v>2.875876E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1764097240</v>
       </c>
@@ -4139,7 +5124,7 @@
         <v>9.7873079999999995E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1764097240</v>
       </c>
@@ -4171,7 +5156,7 @@
         <v>8.9504675999999998E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1764097240</v>
       </c>
@@ -4203,7 +5188,7 @@
         <v>9.8048639999999998E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1764097240</v>
       </c>
@@ -4235,7 +5220,7 @@
         <v>7.0122069999999995E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1764097240</v>
       </c>
@@ -4267,7 +5252,7 @@
         <v>1.3754024E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1764097240</v>
       </c>
@@ -4299,7 +5284,7 @@
         <v>1.0798004999999999E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1764097240</v>
       </c>
@@ -4331,7 +5316,7 @@
         <v>2.0019194999999999E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1764097240</v>
       </c>
@@ -4363,7 +5348,7 @@
         <v>5.3293069999999999E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1764097240</v>
       </c>
@@ -4395,7 +5380,7 @@
         <v>6.2437630000000002E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1764097240</v>
       </c>
@@ -4427,7 +5412,7 @@
         <v>7.9129626E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1764097240</v>
       </c>
@@ -4459,7 +5444,7 @@
         <v>1.4113793E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1764097240</v>
       </c>
@@ -4491,7 +5476,7 @@
         <v>9.6409299999999999E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1764097240</v>
       </c>
@@ -4523,7 +5508,7 @@
         <v>5.4580729999999999E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1764097240</v>
       </c>
@@ -4555,7 +5540,7 @@
         <v>5.62476E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1764097240</v>
       </c>
@@ -4587,7 +5572,7 @@
         <v>5.6132616000000002E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1764097240</v>
       </c>
@@ -4619,7 +5604,7 @@
         <v>7.4005686000000004E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1764097240</v>
       </c>
@@ -4651,7 +5636,7 @@
         <v>1.077843E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1764097240</v>
       </c>
@@ -4683,7 +5668,7 @@
         <v>9.3133800000000006E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1764097240</v>
       </c>
@@ -4715,7 +5700,7 @@
         <v>2.9596435999999999E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1764097240</v>
       </c>
@@ -4747,7 +5732,7 @@
         <v>1.3922808000000001E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1764097240</v>
       </c>
@@ -4779,7 +5764,7 @@
         <v>1.1128099999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1764097240</v>
       </c>
@@ -4811,7 +5796,7 @@
         <v>1.0413584E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1764097240</v>
       </c>
@@ -4843,7 +5828,7 @@
         <v>8.2198865000000001E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1764097240</v>
       </c>
@@ -4875,7 +5860,7 @@
         <v>2.088475E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1764097240</v>
       </c>
@@ -4907,7 +5892,7 @@
         <v>1.0623142E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1764097240</v>
       </c>
@@ -4939,7 +5924,7 @@
         <v>9.3174359999999997E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1764097240</v>
       </c>
@@ -4971,7 +5956,7 @@
         <v>2.1975771000000001E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1764097240</v>
       </c>
@@ -5003,7 +5988,7 @@
         <v>3.9754354999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1764097240</v>
       </c>
@@ -5035,7 +6020,7 @@
         <v>1.9018290999999999E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1764097240</v>
       </c>
@@ -5067,7 +6052,7 @@
         <v>9.6660939999999997E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1764097240</v>
       </c>
@@ -5099,7 +6084,7 @@
         <v>1.0758568E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1764097240</v>
       </c>
@@ -5131,7 +6116,7 @@
         <v>1.3596214E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1764097240</v>
       </c>
@@ -5163,7 +6148,7 @@
         <v>2.7182292E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1764097240</v>
       </c>
@@ -5195,7 +6180,7 @@
         <v>1.6953817E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1764097240</v>
       </c>
@@ -5227,7 +6212,7 @@
         <v>8.8626859999999994E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1764097240</v>
       </c>
@@ -5259,7 +6244,7 @@
         <v>2.2888968E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1764097240</v>
       </c>
@@ -5291,7 +6276,7 @@
         <v>8.3837160000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1764097240</v>
       </c>
@@ -5323,7 +6308,7 @@
         <v>5.6911922E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1764097240</v>
       </c>
@@ -5355,7 +6340,7 @@
         <v>2.768444E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1764097240</v>
       </c>
@@ -5387,7 +6372,7 @@
         <v>6.0429149999999997E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1764097240</v>
       </c>
@@ -5419,7 +6404,7 @@
         <v>1.6286909999999999E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1764097240</v>
       </c>
@@ -5451,7 +6436,7 @@
         <v>5.8010533E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1764097240</v>
       </c>
@@ -5483,7 +6468,7 @@
         <v>8.8111100000000004E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1764097240</v>
       </c>
@@ -5515,7 +6500,7 @@
         <v>9.491216E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1764097240</v>
       </c>
@@ -5547,7 +6532,7 @@
         <v>9.1174250000000002E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1764097240</v>
       </c>
@@ -5579,7 +6564,7 @@
         <v>4.1628780000000002E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1764097240</v>
       </c>
@@ -5611,7 +6596,7 @@
         <v>2.2461509999999999E-6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1764097240</v>
       </c>
@@ -5643,7 +6628,7 @@
         <v>8.8955880000000005E-6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1764097240</v>
       </c>
@@ -5675,7 +6660,7 @@
         <v>4.3820219999999999E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1764097240</v>
       </c>
@@ -5707,7 +6692,7 @@
         <v>6.4562260000000001E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1764097240</v>
       </c>
@@ -5739,7 +6724,7 @@
         <v>5.5779575999999998E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1764097240</v>
       </c>
@@ -5771,7 +6756,7 @@
         <v>2.9899478E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1764097240</v>
       </c>
@@ -5803,7 +6788,7 @@
         <v>1.2692959999999999E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1764097240</v>
       </c>
@@ -5835,7 +6820,7 @@
         <v>2.5627474E-5</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1764097240</v>
       </c>
@@ -5867,7 +6852,7 @@
         <v>3.6372232E-6</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1764097240</v>
       </c>
@@ -5899,7 +6884,7 @@
         <v>3.9940239999999997E-5</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1764097240</v>
       </c>
@@ -5931,7 +6916,7 @@
         <v>1.9990911999999999E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1764097240</v>
       </c>
@@ -5963,7 +6948,7 @@
         <v>6.0188500000000001E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1764097240</v>
       </c>
@@ -5995,7 +6980,7 @@
         <v>9.847042E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1764097240</v>
       </c>
@@ -6027,7 +7012,7 @@
         <v>3.2026690000000002E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1764097240</v>
       </c>
@@ -6059,7 +7044,7 @@
         <v>5.0628976E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1764097240</v>
       </c>
@@ -6091,7 +7076,7 @@
         <v>9.0713209999999998E-5</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1764097240</v>
       </c>
@@ -6123,7 +7108,7 @@
         <v>1.1983829E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1764097240</v>
       </c>
@@ -6155,7 +7140,7 @@
         <v>3.4016266000000002E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1764097240</v>
       </c>
@@ -6187,7 +7172,7 @@
         <v>6.107121E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1764097240</v>
       </c>
@@ -6219,7 +7204,7 @@
         <v>3.1151507000000001E-5</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1764097240</v>
       </c>
@@ -6251,7 +7236,7 @@
         <v>2.4765184000000001E-5</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1764097240</v>
       </c>
@@ -6283,7 +7268,7 @@
         <v>1.4768903999999999E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1764097240</v>
       </c>
@@ -6315,7 +7300,7 @@
         <v>1.3117407999999999E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1764097240</v>
       </c>
@@ -6347,7 +7332,7 @@
         <v>5.7936139999999999E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1764097240</v>
       </c>
@@ -6379,7 +7364,7 @@
         <v>4.9363064999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1764097240</v>
       </c>
@@ -6411,7 +7396,7 @@
         <v>4.7346126000000002E-5</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1764097240</v>
       </c>
@@ -6443,7 +7428,7 @@
         <v>8.0795957000000002E-7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1764097240</v>
       </c>
@@ -6475,7 +7460,7 @@
         <v>6.6751715999999997E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1764097240</v>
       </c>
@@ -6507,7 +7492,7 @@
         <v>1.5566602E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1764097240</v>
       </c>
@@ -6539,7 +7524,7 @@
         <v>4.8924324999999997E-5</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1764097240</v>
       </c>
@@ -6571,7 +7556,7 @@
         <v>1.9435913E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1764097240</v>
       </c>
@@ -6603,7 +7588,7 @@
         <v>1.5087788000000001E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1764097240</v>
       </c>
@@ -6635,7 +7620,7 @@
         <v>9.8831354999999994E-5</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1764097240</v>
       </c>
@@ -6667,7 +7652,7 @@
         <v>3.5824356000000002E-5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1764097240</v>
       </c>
@@ -6699,7 +7684,7 @@
         <v>1.2910189999999999E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1764097240</v>
       </c>
@@ -6731,7 +7716,7 @@
         <v>6.2083025000000003E-5</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1764097240</v>
       </c>
@@ -6763,7 +7748,7 @@
         <v>1.11786256E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1764097240</v>
       </c>
@@ -6795,7 +7780,7 @@
         <v>2.2681514000000001E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1764097240</v>
       </c>
@@ -6827,7 +7812,7 @@
         <v>1.2199694E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1764097240</v>
       </c>
@@ -6859,7 +7844,7 @@
         <v>9.3134150000000003E-5</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1764097240</v>
       </c>
@@ -6891,7 +7876,7 @@
         <v>1.4528625000000001E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1764097240</v>
       </c>
@@ -6923,7 +7908,7 @@
         <v>1.4258926E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1764097240</v>
       </c>
@@ -6955,7 +7940,7 @@
         <v>4.4078726E-5</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1764097240</v>
       </c>
@@ -6987,7 +7972,7 @@
         <v>1.09381836E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1764097240</v>
       </c>
@@ -7019,7 +8004,7 @@
         <v>4.0007642000000001E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1764097240</v>
       </c>
@@ -7051,7 +8036,7 @@
         <v>1.8105142E-4</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1764097240</v>
       </c>
@@ -7083,7 +8068,7 @@
         <v>4.9938254999999999E-5</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1764097240</v>
       </c>
@@ -7115,7 +8100,7 @@
         <v>7.6996999999999995E-5</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>1764097240</v>
       </c>
@@ -7147,7 +8132,7 @@
         <v>5.2661377000000001E-5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1764097240</v>
       </c>
@@ -7179,7 +8164,7 @@
         <v>3.5664390000000003E-5</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1764097240</v>
       </c>
@@ -7211,7 +8196,7 @@
         <v>1.0879894400000001E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1764097240</v>
       </c>
@@ -7243,7 +8228,7 @@
         <v>1.0299820000000001E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1764097240</v>
       </c>
@@ -7275,7 +8260,7 @@
         <v>1.0318593999999999E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1764097240</v>
       </c>
@@ -7307,7 +8292,7 @@
         <v>7.1215200000000002E-5</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1764097240</v>
       </c>
@@ -7339,7 +8324,7 @@
         <v>1.4807598999999999E-5</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1764097240</v>
       </c>
@@ -7371,7 +8356,7 @@
         <v>2.8349262999999999E-5</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1764097240</v>
       </c>
@@ -7403,7 +8388,7 @@
         <v>8.4142059999999999E-5</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>1764097240</v>
       </c>
@@ -7435,7 +8420,7 @@
         <v>8.2307789999999998E-5</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1764097240</v>
       </c>
@@ -7467,7 +8452,7 @@
         <v>6.9160860000000001E-5</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1764097240</v>
       </c>
@@ -7499,7 +8484,7 @@
         <v>1.0219902E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1764097240</v>
       </c>
@@ -7531,7 +8516,7 @@
         <v>1.7601902E-4</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1764097240</v>
       </c>
@@ -7563,7 +8548,7 @@
         <v>8.8468599999999995E-5</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1764097240</v>
       </c>
@@ -7595,7 +8580,7 @@
         <v>6.9884575999999999E-5</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>1764097240</v>
       </c>
@@ -7627,7 +8612,7 @@
         <v>1.4915026E-5</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1764097240</v>
       </c>
@@ -7659,7 +8644,7 @@
         <v>3.4995086000000001E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1764097240</v>
       </c>
@@ -7691,7 +8676,7 @@
         <v>4.8669523999999998E-5</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1764097240</v>
       </c>
@@ -7723,7 +8708,7 @@
         <v>7.0124300000000002E-5</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1764097240</v>
       </c>
@@ -7755,7 +8740,7 @@
         <v>7.1770660000000004E-5</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1764097240</v>
       </c>
@@ -7787,7 +8772,7 @@
         <v>8.1727769999999998E-5</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1764097240</v>
       </c>
@@ -7819,7 +8804,7 @@
         <v>7.7496800000000007E-5</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1764097240</v>
       </c>
@@ -7851,7 +8836,7 @@
         <v>1.2961782000000001E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>1764097240</v>
       </c>
@@ -7883,7 +8868,7 @@
         <v>1.05599334E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>1764097240</v>
       </c>
@@ -7915,7 +8900,7 @@
         <v>6.1715200000000002E-5</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>1764097240</v>
       </c>
@@ -7947,7 +8932,7 @@
         <v>5.9913269999999999E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1764097240</v>
       </c>
@@ -7979,7 +8964,7 @@
         <v>3.6500210000000001E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>1764097240</v>
       </c>
@@ -8011,7 +8996,7 @@
         <v>7.3036470000000002E-5</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>1764097240</v>
       </c>
@@ -8043,7 +9028,7 @@
         <v>1.0329631E-4</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>1764097240</v>
       </c>
@@ -8075,7 +9060,7 @@
         <v>1.4747585000000001E-4</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>1764097240</v>
       </c>
@@ -8107,7 +9092,7 @@
         <v>1.3596349000000001E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>1764097240</v>
       </c>
@@ -8139,7 +9124,7 @@
         <v>8.7447180000000004E-5</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>1764097240</v>
       </c>
@@ -8171,7 +9156,7 @@
         <v>2.7315009999999999E-5</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>1764097240</v>
       </c>
@@ -8203,7 +9188,7 @@
         <v>2.4686145E-5</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>1764097240</v>
       </c>
@@ -8235,7 +9220,7 @@
         <v>1.7485273000000001E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>1764097240</v>
       </c>
@@ -8267,7 +9252,7 @@
         <v>1.2907629E-4</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>1764097240</v>
       </c>
@@ -8299,7 +9284,7 @@
         <v>4.1231820000000002E-5</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>1764097240</v>
       </c>
@@ -8331,7 +9316,7 @@
         <v>4.9753777000000002E-5</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>1764097240</v>
       </c>
@@ -8363,7 +9348,7 @@
         <v>7.5051857E-6</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>1764097240</v>
       </c>
@@ -8395,7 +9380,7 @@
         <v>3.0321414999999998E-5</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>1764097240</v>
       </c>
@@ -8427,7 +9412,7 @@
         <v>1.1328743999999999E-5</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>1764097240</v>
       </c>
@@ -8459,7 +9444,7 @@
         <v>1.7208747000000001E-4</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>1764097240</v>
       </c>
@@ -8491,7 +9476,7 @@
         <v>1.2459164999999999E-4</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>1764097240</v>
       </c>
@@ -8523,7 +9508,7 @@
         <v>7.6680699999999999E-5</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>1764097240</v>
       </c>
@@ -8555,7 +9540,7 @@
         <v>1.4476826E-4</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>1764097240</v>
       </c>
@@ -8587,7 +9572,7 @@
         <v>2.1814722999999999E-5</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>1764097240</v>
       </c>
@@ -8619,7 +9604,7 @@
         <v>4.244377E-5</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>1764097240</v>
       </c>
@@ -8651,7 +9636,7 @@
         <v>6.1230999999999997E-5</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>1764097240</v>
       </c>
@@ -8683,7 +9668,7 @@
         <v>7.3160050000000001E-5</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>1764097240</v>
       </c>
@@ -8715,7 +9700,7 @@
         <v>2.0036937999999998E-5</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>1764097240</v>
       </c>
@@ -8747,7 +9732,7 @@
         <v>5.5362226999999997E-5</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>1764097240</v>
       </c>
@@ -8779,7 +9764,7 @@
         <v>8.1246879999999995E-5</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>1764097240</v>
       </c>
@@ -8811,7 +9796,7 @@
         <v>1.1979643000000001E-5</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>1764097240</v>
       </c>
@@ -8843,7 +9828,7 @@
         <v>8.990983E-5</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>1764097240</v>
       </c>
@@ -8875,7 +9860,7 @@
         <v>7.1742639999999996E-5</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>1764097240</v>
       </c>
@@ -8907,7 +9892,7 @@
         <v>8.9984820000000001E-5</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>1764097240</v>
       </c>
@@ -8939,7 +9924,7 @@
         <v>7.1951479999999996E-5</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>1764097240</v>
       </c>
@@ -8971,7 +9956,7 @@
         <v>7.6987010000000001E-5</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>1764097240</v>
       </c>
@@ -9003,7 +9988,7 @@
         <v>7.7718230000000006E-5</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>1764097240</v>
       </c>
@@ -9035,7 +10020,7 @@
         <v>9.5114749999999996E-5</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>1764097240</v>
       </c>
@@ -9067,7 +10052,7 @@
         <v>1.05691564E-4</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>1764097240</v>
       </c>
@@ -9099,7 +10084,7 @@
         <v>9.5301309999999996E-5</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>1764097240</v>
       </c>
@@ -9131,7 +10116,7 @@
         <v>6.8996814999999997E-5</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>1764097240</v>
       </c>
@@ -9163,7 +10148,7 @@
         <v>3.0311366999999999E-5</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>1764097240</v>
       </c>
@@ -9193,6 +10178,45 @@
       </c>
       <c r="J163" s="1">
         <v>5.6852889999999998E-5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>1764097240</v>
+      </c>
+      <c r="B164" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" t="s">
+        <v>10</v>
+      </c>
+      <c r="D164">
+        <f>AVERAGE(D2:D163)</f>
+        <v>674880</v>
+      </c>
+      <c r="E164">
+        <f t="shared" ref="E164:J164" si="0">AVERAGE(E2:E163)</f>
+        <v>1244160</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="0"/>
+        <v>0.51015970000000133</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="0"/>
+        <v>0.49826989999999821</v>
+      </c>
+      <c r="H164">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="0"/>
+        <v>2.4455743243827158E-3</v>
+      </c>
+      <c r="J164">
+        <f t="shared" si="0"/>
+        <v>7.1222183755987657E-5</v>
       </c>
     </row>
   </sheetData>
@@ -9202,27 +10226,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EFDFA6-3EAC-43FB-8076-C79ADDE20907}">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="B144" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9254,7 +10278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1764097240</v>
       </c>
@@ -9286,7 +10310,7 @@
         <v>1.9998354999999998E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1764097240</v>
       </c>
@@ -9318,7 +10342,7 @@
         <v>6.2686100000000003E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1764097240</v>
       </c>
@@ -9350,7 +10374,7 @@
         <v>1.2141819999999999E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1764097240</v>
       </c>
@@ -9382,7 +10406,7 @@
         <v>4.2174976000000003E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1764097240</v>
       </c>
@@ -9414,7 +10438,7 @@
         <v>3.6498244000000003E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1764097240</v>
       </c>
@@ -9446,7 +10470,7 @@
         <v>3.6316049999999999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1764097240</v>
       </c>
@@ -9478,7 +10502,7 @@
         <v>2.9017520999999999E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1764097240</v>
       </c>
@@ -9510,7 +10534,7 @@
         <v>5.9567549999999999E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1764097240</v>
       </c>
@@ -9542,7 +10566,7 @@
         <v>5.7336749999999998E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1764097240</v>
       </c>
@@ -9574,7 +10598,7 @@
         <v>1.0015328E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1764097240</v>
       </c>
@@ -9606,7 +10630,7 @@
         <v>3.6416776999999998E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1764097240</v>
       </c>
@@ -9638,7 +10662,7 @@
         <v>2.5729358E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1764097240</v>
       </c>
@@ -9670,7 +10694,7 @@
         <v>3.3642980000000002E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1764097240</v>
       </c>
@@ -9702,7 +10726,7 @@
         <v>5.7071160000000001E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1764097240</v>
       </c>
@@ -9734,7 +10758,7 @@
         <v>4.0759754000000003E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1764097240</v>
       </c>
@@ -9766,7 +10790,7 @@
         <v>2.1012923999999999E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1764097240</v>
       </c>
@@ -9798,7 +10822,7 @@
         <v>2.8227529E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1764097240</v>
       </c>
@@ -9830,7 +10854,7 @@
         <v>2.1762233E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1764097240</v>
       </c>
@@ -9862,7 +10886,7 @@
         <v>3.3885130000000001E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1764097240</v>
       </c>
@@ -9894,7 +10918,7 @@
         <v>4.8743794000000003E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1764097240</v>
       </c>
@@ -9926,7 +10950,7 @@
         <v>4.0154936999999999E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1764097240</v>
       </c>
@@ -9958,7 +10982,7 @@
         <v>1.2311267999999999E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1764097240</v>
       </c>
@@ -9990,7 +11014,7 @@
         <v>5.7462876000000003E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1764097240</v>
       </c>
@@ -10022,7 +11046,7 @@
         <v>4.2963799999999997E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1764097240</v>
       </c>
@@ -10054,7 +11078,7 @@
         <v>4.174867E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1764097240</v>
       </c>
@@ -10086,7 +11110,7 @@
         <v>3.0877996000000001E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1764097240</v>
       </c>
@@ -10118,7 +11142,7 @@
         <v>9.0054069999999993E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1764097240</v>
       </c>
@@ -10150,7 +11174,7 @@
         <v>5.0255315999999997E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1764097240</v>
       </c>
@@ -10182,7 +11206,7 @@
         <v>3.7746690000000002E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1764097240</v>
       </c>
@@ -10214,7 +11238,7 @@
         <v>6.8152017000000002E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1764097240</v>
       </c>
@@ -10246,7 +11270,7 @@
         <v>1.2629703E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1764097240</v>
       </c>
@@ -10278,7 +11302,7 @@
         <v>7.3134825E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1764097240</v>
       </c>
@@ -10310,7 +11334,7 @@
         <v>3.6559366000000001E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1764097240</v>
       </c>
@@ -10342,7 +11366,7 @@
         <v>4.3455689999999997E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1764097240</v>
       </c>
@@ -10374,7 +11398,7 @@
         <v>5.1332535999999999E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1764097240</v>
       </c>
@@ -10406,7 +11430,7 @@
         <v>1.20255445E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1764097240</v>
       </c>
@@ -10438,7 +11462,7 @@
         <v>7.0226440000000005E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1764097240</v>
       </c>
@@ -10470,7 +11494,7 @@
         <v>3.7962693999999998E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1764097240</v>
       </c>
@@ -10502,7 +11526,7 @@
         <v>6.6902817000000002E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1764097240</v>
       </c>
@@ -10534,7 +11558,7 @@
         <v>3.5106476999999997E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1764097240</v>
       </c>
@@ -10566,7 +11590,7 @@
         <v>1.8607321000000001E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1764097240</v>
       </c>
@@ -10598,7 +11622,7 @@
         <v>1.4914442000000001E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1764097240</v>
       </c>
@@ -10630,7 +11654,7 @@
         <v>2.3780324999999998E-5</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1764097240</v>
       </c>
@@ -10662,7 +11686,7 @@
         <v>4.71297E-6</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1764097240</v>
       </c>
@@ -10694,7 +11718,7 @@
         <v>2.1492676999999999E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1764097240</v>
       </c>
@@ -10726,7 +11750,7 @@
         <v>3.4229600000000002E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1764097240</v>
       </c>
@@ -10758,7 +11782,7 @@
         <v>3.5207453000000003E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1764097240</v>
       </c>
@@ -10790,7 +11814,7 @@
         <v>3.3403969999999999E-6</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1764097240</v>
       </c>
@@ -10822,7 +11846,7 @@
         <v>1.9243900000000001E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1764097240</v>
       </c>
@@ -10854,7 +11878,7 @@
         <v>1.1426531E-6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1764097240</v>
       </c>
@@ -10886,7 +11910,7 @@
         <v>3.6876965999999998E-6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1764097240</v>
       </c>
@@ -10918,7 +11942,7 @@
         <v>1.9831E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1764097240</v>
       </c>
@@ -10950,7 +11974,7 @@
         <v>2.5910839999999999E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1764097240</v>
       </c>
@@ -10982,7 +12006,7 @@
         <v>1.9761824999999999E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1764097240</v>
       </c>
@@ -11014,7 +12038,7 @@
         <v>1.2478895E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1764097240</v>
       </c>
@@ -11046,7 +12070,7 @@
         <v>4.0630083999999999E-6</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1764097240</v>
       </c>
@@ -11078,7 +12102,7 @@
         <v>7.370624E-6</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1764097240</v>
       </c>
@@ -11110,7 +12134,7 @@
         <v>1.5253325999999999E-6</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1764097240</v>
       </c>
@@ -11142,7 +12166,7 @@
         <v>1.3945309E-5</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1764097240</v>
       </c>
@@ -11174,7 +12198,7 @@
         <v>7.7912823999999996E-5</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1764097240</v>
       </c>
@@ -11206,7 +12230,7 @@
         <v>2.1798238000000001E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1764097240</v>
       </c>
@@ -11238,7 +12262,7 @@
         <v>4.2123735E-5</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1764097240</v>
       </c>
@@ -11270,7 +12294,7 @@
         <v>1.5209068000000001E-5</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1764097240</v>
       </c>
@@ -11302,7 +12326,7 @@
         <v>1.9465503999999999E-5</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1764097240</v>
       </c>
@@ -11334,7 +12358,7 @@
         <v>3.7035274999999999E-5</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1764097240</v>
       </c>
@@ -11366,7 +12390,7 @@
         <v>3.1110675999999999E-6</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1764097240</v>
       </c>
@@ -11398,7 +12422,7 @@
         <v>8.8230899999999996E-6</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1764097240</v>
       </c>
@@ -11430,7 +12454,7 @@
         <v>2.7242929999999998E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1764097240</v>
       </c>
@@ -11462,7 +12486,7 @@
         <v>1.3361436000000001E-5</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1764097240</v>
       </c>
@@ -11494,7 +12518,7 @@
         <v>8.2826854999999998E-6</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1764097240</v>
       </c>
@@ -11526,7 +12550,7 @@
         <v>4.4795056E-6</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1764097240</v>
       </c>
@@ -11558,7 +12582,7 @@
         <v>5.1095930000000002E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1764097240</v>
       </c>
@@ -11590,7 +12614,7 @@
         <v>2.2614217000000001E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1764097240</v>
       </c>
@@ -11622,7 +12646,7 @@
         <v>2.3352914999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1764097240</v>
       </c>
@@ -11654,7 +12678,7 @@
         <v>1.8708197E-5</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1764097240</v>
       </c>
@@ -11686,7 +12710,7 @@
         <v>6.0923185000000005E-7</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1764097240</v>
       </c>
@@ -11718,7 +12742,7 @@
         <v>2.1848656999999999E-5</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1764097240</v>
       </c>
@@ -11750,7 +12774,7 @@
         <v>6.2361386999999997E-6</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1764097240</v>
       </c>
@@ -11782,7 +12806,7 @@
         <v>2.2617238000000002E-5</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1764097240</v>
       </c>
@@ -11814,7 +12838,7 @@
         <v>8.1838639999999995E-6</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1764097240</v>
       </c>
@@ -11846,7 +12870,7 @@
         <v>5.9987076000000001E-5</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1764097240</v>
       </c>
@@ -11878,7 +12902,7 @@
         <v>4.3018776000000003E-5</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1764097240</v>
       </c>
@@ -11910,7 +12934,7 @@
         <v>1.5992333E-5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1764097240</v>
       </c>
@@ -11942,7 +12966,7 @@
         <v>5.4182757999999997E-5</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1764097240</v>
       </c>
@@ -11974,7 +12998,7 @@
         <v>2.6733663999999999E-5</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1764097240</v>
       </c>
@@ -12006,7 +13030,7 @@
         <v>4.5177070000000003E-5</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1764097240</v>
       </c>
@@ -12038,7 +13062,7 @@
         <v>9.4275279999999994E-5</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1764097240</v>
       </c>
@@ -12070,7 +13094,7 @@
         <v>5.1161627000000002E-5</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1764097240</v>
       </c>
@@ -12102,7 +13126,7 @@
         <v>3.7494899999999999E-5</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1764097240</v>
       </c>
@@ -12134,7 +13158,7 @@
         <v>6.0559327000000002E-5</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1764097240</v>
       </c>
@@ -12166,7 +13190,7 @@
         <v>5.6616424000000001E-5</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1764097240</v>
       </c>
@@ -12198,7 +13222,7 @@
         <v>1.7458975000000002E-5</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1764097240</v>
       </c>
@@ -12230,7 +13254,7 @@
         <v>4.5736735000000001E-5</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1764097240</v>
       </c>
@@ -12262,7 +13286,7 @@
         <v>1.422621E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1764097240</v>
       </c>
@@ -12294,7 +13318,7 @@
         <v>7.9343489999999996E-5</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1764097240</v>
       </c>
@@ -12326,7 +13350,7 @@
         <v>1.8791013999999998E-5</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1764097240</v>
       </c>
@@ -12358,7 +13382,7 @@
         <v>3.2949883000000001E-5</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>1764097240</v>
       </c>
@@ -12390,7 +13414,7 @@
         <v>1.8265879999999999E-5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1764097240</v>
       </c>
@@ -12422,7 +13446,7 @@
         <v>1.3118680000000001E-5</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>1764097240</v>
       </c>
@@ -12454,7 +13478,7 @@
         <v>4.4206826999999999E-5</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1764097240</v>
       </c>
@@ -12486,7 +13510,7 @@
         <v>3.9910290000000002E-5</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>1764097240</v>
       </c>
@@ -12518,7 +13542,7 @@
         <v>4.3643773000000003E-5</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1764097240</v>
       </c>
@@ -12550,7 +13574,7 @@
         <v>2.9938758000000001E-5</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>1764097240</v>
       </c>
@@ -12582,7 +13606,7 @@
         <v>8.5261949999999994E-6</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1764097240</v>
       </c>
@@ -12614,7 +13638,7 @@
         <v>1.205744E-5</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1764097240</v>
       </c>
@@ -12646,7 +13670,7 @@
         <v>3.348633E-5</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>1764097240</v>
       </c>
@@ -12678,7 +13702,7 @@
         <v>3.381266E-5</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1764097240</v>
       </c>
@@ -12710,7 +13734,7 @@
         <v>2.9602986999999999E-5</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>1764097240</v>
       </c>
@@ -12742,7 +13766,7 @@
         <v>4.6850369999999999E-5</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1764097240</v>
       </c>
@@ -12774,7 +13798,7 @@
         <v>7.1435876000000006E-5</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>1764097240</v>
       </c>
@@ -12806,7 +13830,7 @@
         <v>3.5054156E-5</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1764097240</v>
       </c>
@@ -12838,7 +13862,7 @@
         <v>3.1658105999999997E-5</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>1764097240</v>
       </c>
@@ -12870,7 +13894,7 @@
         <v>5.3783650000000001E-6</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1764097240</v>
       </c>
@@ -12902,7 +13926,7 @@
         <v>1.5591322000000001E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>1764097240</v>
       </c>
@@ -12934,7 +13958,7 @@
         <v>1.9243906E-5</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1764097240</v>
       </c>
@@ -12966,7 +13990,7 @@
         <v>3.0025430000000001E-5</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1764097240</v>
       </c>
@@ -12998,7 +14022,7 @@
         <v>2.5991605000000001E-5</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>1764097240</v>
       </c>
@@ -13030,7 +14054,7 @@
         <v>3.1998359999999999E-5</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1764097240</v>
       </c>
@@ -13062,7 +14086,7 @@
         <v>3.2108964999999998E-5</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>1764097240</v>
       </c>
@@ -13094,7 +14118,7 @@
         <v>5.1093980000000001E-5</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>1764097240</v>
       </c>
@@ -13126,7 +14150,7 @@
         <v>4.4429489999999998E-5</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>1764097240</v>
       </c>
@@ -13158,7 +14182,7 @@
         <v>2.8741861999999999E-5</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>1764097240</v>
       </c>
@@ -13190,7 +14214,7 @@
         <v>2.4625470000000001E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1764097240</v>
       </c>
@@ -13222,7 +14246,7 @@
         <v>1.3108425999999999E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>1764097240</v>
       </c>
@@ -13254,7 +14278,7 @@
         <v>2.8913038E-5</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>1764097240</v>
       </c>
@@ -13286,7 +14310,7 @@
         <v>4.0056657000000001E-5</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>1764097240</v>
       </c>
@@ -13318,7 +14342,7 @@
         <v>5.0958965999999998E-5</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>1764097240</v>
       </c>
@@ -13350,7 +14374,7 @@
         <v>5.0541670000000002E-5</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>1764097240</v>
       </c>
@@ -13382,7 +14406,7 @@
         <v>3.4568576999999997E-5</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>1764097240</v>
       </c>
@@ -13414,7 +14438,7 @@
         <v>9.656299E-6</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>1764097240</v>
       </c>
@@ -13446,7 +14470,7 @@
         <v>9.654788E-6</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>1764097240</v>
       </c>
@@ -13478,7 +14502,7 @@
         <v>6.5764259999999994E-5</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>1764097240</v>
       </c>
@@ -13510,7 +14534,7 @@
         <v>5.7435256000000002E-5</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>1764097240</v>
       </c>
@@ -13542,7 +14566,7 @@
         <v>1.2301013E-5</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>1764097240</v>
       </c>
@@ -13574,7 +14598,7 @@
         <v>1.8054682999999999E-5</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>1764097240</v>
       </c>
@@ -13606,7 +14630,7 @@
         <v>2.4060735000000001E-6</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>1764097240</v>
       </c>
@@ -13638,7 +14662,7 @@
         <v>1.2684739000000001E-5</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>1764097240</v>
       </c>
@@ -13670,7 +14694,7 @@
         <v>5.0555519999999999E-6</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>1764097240</v>
       </c>
@@ -13702,7 +14726,7 @@
         <v>6.6364279999999996E-5</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>1764097240</v>
       </c>
@@ -13734,7 +14758,7 @@
         <v>4.7174842999999999E-5</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>1764097240</v>
       </c>
@@ -13766,7 +14790,7 @@
         <v>2.7033317000000001E-5</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>1764097240</v>
       </c>
@@ -13798,7 +14822,7 @@
         <v>5.6759596E-5</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>1764097240</v>
       </c>
@@ -13830,7 +14854,7 @@
         <v>7.4549353000000001E-6</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>1764097240</v>
       </c>
@@ -13862,7 +14886,7 @@
         <v>1.9149444E-5</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>1764097240</v>
       </c>
@@ -13894,7 +14918,7 @@
         <v>1.5902837000000001E-5</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>1764097240</v>
       </c>
@@ -13926,7 +14950,7 @@
         <v>2.9349235999999999E-5</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>1764097240</v>
       </c>
@@ -13958,7 +14982,7 @@
         <v>6.0320300000000004E-6</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>1764097240</v>
       </c>
@@ -13990,7 +15014,7 @@
         <v>2.0681871E-5</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>1764097240</v>
       </c>
@@ -14022,7 +15046,7 @@
         <v>3.4171763999999999E-5</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>1764097240</v>
       </c>
@@ -14054,7 +15078,7 @@
         <v>7.0030496E-6</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>1764097240</v>
       </c>
@@ -14086,7 +15110,7 @@
         <v>3.6858927999999997E-5</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>1764097240</v>
       </c>
@@ -14118,7 +15142,7 @@
         <v>2.8281633000000001E-5</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>1764097240</v>
       </c>
@@ -14150,7 +15174,7 @@
         <v>3.8737245999999998E-5</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>1764097240</v>
       </c>
@@ -14182,7 +15206,7 @@
         <v>2.9135711999999999E-5</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>1764097240</v>
       </c>
@@ -14214,7 +15238,7 @@
         <v>2.8445154000000001E-5</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>1764097240</v>
       </c>
@@ -14246,7 +15270,7 @@
         <v>3.21461E-5</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>1764097240</v>
       </c>
@@ -14278,7 +15302,7 @@
         <v>4.1988940000000003E-5</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>1764097240</v>
       </c>
@@ -14310,7 +15334,7 @@
         <v>4.2902665999999999E-5</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>1764097240</v>
       </c>
@@ -14342,7 +15366,7 @@
         <v>4.3733565999999998E-5</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>1764097240</v>
       </c>
@@ -14374,7 +15398,7 @@
         <v>2.9387737000000001E-5</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>1764097240</v>
       </c>
@@ -14406,7 +15430,7 @@
         <v>1.1163596E-5</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>1764097240</v>
       </c>
@@ -14436,6 +15460,45 @@
       </c>
       <c r="J163" s="1">
         <v>2.1962899999999999E-5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>1764097240</v>
+      </c>
+      <c r="B164" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164">
+        <f>AVERAGE(D2:D163)</f>
+        <v>701641</v>
+      </c>
+      <c r="E164">
+        <f t="shared" ref="E164:J164" si="0">AVERAGE(E2:E163)</f>
+        <v>1244148</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="0"/>
+        <v>0.53038899999999967</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="0"/>
+        <v>0.49826509999999874</v>
+      </c>
+      <c r="H164">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I164">
+        <f t="shared" si="0"/>
+        <v>2.6649133732098776E-4</v>
+      </c>
+      <c r="J164">
+        <f t="shared" si="0"/>
+        <v>2.8784700291666677E-5</v>
       </c>
     </row>
   </sheetData>
@@ -14447,11 +15510,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78BA790-5E7D-4543-A39B-EC57BD9C767B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView topLeftCell="A28" zoomScale="83" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD54" sqref="AD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>